<commit_message>
update phân quyền và tạo bài thi
</commit_message>
<xml_diff>
--- a/backend/core/static/files/file mẫu giám khảo.xlsx
+++ b/backend/core/static/files/file mẫu giám khảo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trong\Documents\fpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76A31AF-CCA6-48C5-8096-CE243CB79010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63C5384-8746-4AF9-99C2-BE934939858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3EAE9C44-F124-4E56-A46D-9D98FD06C90F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MaNV</t>
   </si>
@@ -52,12 +52,18 @@
   <si>
     <t>Nguyen Van A</t>
   </si>
+  <si>
+    <t>Lưu ý: 
+- Vui lòng nhập đầy đủ các trường thông tin
+- Thông tin trên bảng là ví dụ, có thể xóa
+- Trước khi import file, hãy xóa lưu ý này</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +104,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,8 +125,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,12 +155,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -158,6 +186,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -494,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D7DC7C-54EC-4CDF-ACFE-8E5FFF020620}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,7 +547,7 @@
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -518,7 +558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>835165</v>
       </c>
@@ -528,73 +568,114 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:I6"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{6841B57D-F91F-4CAF-A4C1-D7D0190A934E}"/>
   </hyperlinks>

</xml_diff>